<commit_message>
Updating core ETL engine to TSEEQ v6.0.2 Signed-off-by: qlikperf <jrs@qlik.com>
</commit_message>
<xml_diff>
--- a/TSEEQ/Source Documents/TSEEQ Sales Sample/Variables/Sales Dashboard Chart Dimensions.xlsx
+++ b/TSEEQ/Source Documents/TSEEQ Sales Sample/Variables/Sales Dashboard Chart Dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TSEEQ\Source Documents\TSEEQ Sales Sample\Variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tc\EEE\TSEEQ.github_5\Source Documents\TSEEQ Sales Sample\Variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6284DD1-24E0-49D4-A759-71814A7EB27A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD854AC-DB69-4534-97F8-08EB21B49D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{5F9F463C-5202-41FA-8ABC-C69595410BDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F9F463C-5202-41FA-8ABC-C69595410BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Dimension</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Shipper</t>
-  </si>
-  <si>
-    <t>Shipper Name</t>
   </si>
   <si>
     <t>Lowest Dim Allowed</t>
@@ -644,7 +641,7 @@
   <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -764,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>

</xml_diff>